<commit_message>
[REF] Refactoriza por completo el código para crear notas de crédito
</commit_message>
<xml_diff>
--- a/Invoices/files/NC/nc_invoices.xlsx
+++ b/Invoices/files/NC/nc_invoices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\wb_odoo_external_api\Invoices\files\NC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D2E0CC-CCFC-466E-8B1C-4DFD60C6CCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543435B4-3DA3-4F0E-A818-354F54DE85B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5D941F05-6685-4D6A-8FCD-7985621E4B9D}"/>
+    <workbookView xWindow="40860" yWindow="-4905" windowWidth="29040" windowHeight="15990" xr2:uid="{5D941F05-6685-4D6A-8FCD-7985621E4B9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>invoice_id</t>
+    <t>so_origin</t>
   </si>
   <si>
-    <t>726164</t>
+    <t>SO2385027</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>